<commit_message>
Had the wrong tab name for one of the tabs (forgot to have the "d" in "herbivoreData" capitalized)
</commit_message>
<xml_diff>
--- a/Test Data/Shiny Test Data.xlsx
+++ b/Test Data/Shiny Test Data.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick.lyon/Documents/Jobs/2021_HerbVar Network Admin/HerbVar-Data-Portal/Test Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B49EAA6-9D9C-884D-B48C-20E0C1D64FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE30347-6236-3942-A919-C66EFF2044EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-46140" yWindow="5320" windowWidth="28040" windowHeight="17040" activeTab="6" xr2:uid="{75175CB1-0094-B143-8246-DA8391BF8CEA}"/>
+    <workbookView xWindow="-46140" yWindow="5320" windowWidth="28040" windowHeight="17040" activeTab="4" xr2:uid="{75175CB1-0094-B143-8246-DA8391BF8CEA}"/>
   </bookViews>
   <sheets>
     <sheet name="siteData" sheetId="1" r:id="rId1"/>
     <sheet name="densityData" sheetId="3" r:id="rId2"/>
     <sheet name="plantData" sheetId="4" r:id="rId3"/>
     <sheet name="reproData" sheetId="5" r:id="rId4"/>
-    <sheet name="herbivoredata" sheetId="6" r:id="rId5"/>
+    <sheet name="herbivoreData" sheetId="6" r:id="rId5"/>
     <sheet name="newColumns" sheetId="7" r:id="rId6"/>
     <sheet name="notes" sheetId="8" r:id="rId7"/>
   </sheets>
@@ -643,10 +643,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F942DFF-2872-674D-B810-28E9EBD84B24}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B3" sqref="B3"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -741,7 +741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{614E6276-CB20-7040-B561-DB3DD6FF9881}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B3" sqref="B3"/>
       <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>

</xml_diff>